<commit_message>
Added prob4a excel file
</commit_message>
<xml_diff>
--- a/bioalgorithms/hw2/Prob4a.xlsx
+++ b/bioalgorithms/hw2/Prob4a.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="23">
   <si>
     <t>w</t>
   </si>
@@ -112,13 +112,22 @@
     <t>↘.</t>
   </si>
   <si>
-    <t>InDel</t>
-  </si>
-  <si>
     <t>Match</t>
   </si>
   <si>
     <t>Mismatch</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T </t>
+  </si>
+  <si>
+    <t>InDel (insert w)</t>
+  </si>
+  <si>
+    <t>InDel (insert v)</t>
   </si>
 </sst>
 </file>
@@ -510,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,9 +538,21 @@
     <col min="10" max="10" width="4" customWidth="1"/>
     <col min="11" max="11" width="4.77734375" customWidth="1"/>
     <col min="15" max="15" width="15.77734375" customWidth="1"/>
+    <col min="16" max="16" width="6.109375" customWidth="1"/>
+    <col min="17" max="17" width="6" customWidth="1"/>
+    <col min="18" max="18" width="4.44140625" customWidth="1"/>
+    <col min="19" max="19" width="5" customWidth="1"/>
+    <col min="20" max="21" width="4.77734375" customWidth="1"/>
+    <col min="22" max="22" width="5.109375" customWidth="1"/>
+    <col min="23" max="24" width="5.33203125" customWidth="1"/>
+    <col min="25" max="25" width="5.5546875" customWidth="1"/>
+    <col min="26" max="26" width="5.44140625" customWidth="1"/>
+    <col min="27" max="27" width="5.109375" customWidth="1"/>
+    <col min="28" max="28" width="4.44140625" customWidth="1"/>
+    <col min="29" max="29" width="4.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -564,7 +585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -599,7 +620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -634,7 +655,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -669,7 +690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -704,7 +725,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -739,7 +760,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -774,7 +795,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -809,7 +830,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -844,7 +865,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -879,7 +900,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -914,7 +935,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>0</v>
@@ -946,8 +967,44 @@
       <c r="K13" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="T13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="U13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="V13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="W13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="X13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC13" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -981,8 +1038,47 @@
       <c r="K14" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.4">
+      <c r="Q14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
@@ -1020,10 +1116,49 @@
         <v>14</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.4">
+        <v>21</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
@@ -1061,7 +1196,7 @@
         <v>13</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.4">
@@ -1102,7 +1237,7 @@
         <v>15</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.4">
@@ -1143,7 +1278,7 @@
         <v>16</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.4">

</xml_diff>